<commit_message>
removed junk second sheet
</commit_message>
<xml_diff>
--- a/instructions.xlsx
+++ b/instructions.xlsx
@@ -4,11 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="0" windowWidth="24760" windowHeight="20020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,115 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="43">
-  <si>
-    <t>foreigners are niet zo intelligent als irish</t>
-  </si>
-  <si>
-    <t>irish are niet zo intelligent als foreigners</t>
-  </si>
-  <si>
-    <t>irish are intelligenter than foreigners</t>
-  </si>
-  <si>
-    <t>irish are slimmer than foreigners</t>
-  </si>
-  <si>
-    <t>irish are verstandiger than foreigners</t>
-  </si>
-  <si>
-    <t>irish are scherpzinniger than foreigners</t>
-  </si>
-  <si>
-    <t>irish are minder dom than foreigners</t>
-  </si>
-  <si>
-    <t>foreigners are dommer than irish</t>
-  </si>
-  <si>
-    <t>foreigners are minder verstandig than irish</t>
-  </si>
-  <si>
-    <t>foreigners are minder scherpzinnig than irish</t>
-  </si>
-  <si>
-    <t>foreigners are achterlijker than irish</t>
-  </si>
-  <si>
-    <t>irish are dommer than foreigners</t>
-  </si>
-  <si>
-    <t>irish are minder verstandig than foreigners</t>
-  </si>
-  <si>
-    <t>irish are minder scherpzinnig than foreigners</t>
-  </si>
-  <si>
-    <t>irish are achterlijker than foreigners</t>
-  </si>
-  <si>
-    <t>foreigners are intelligenter than irish</t>
-  </si>
-  <si>
-    <t>foreigners are slimmer than irish</t>
-  </si>
-  <si>
-    <t>foreigners are verstandiger than irish</t>
-  </si>
-  <si>
-    <t>foreigners are scherpzinniger than irish</t>
-  </si>
-  <si>
-    <t>foreigners are minder dom than irish</t>
-  </si>
-  <si>
-    <t>irish</t>
-  </si>
-  <si>
-    <t>are</t>
-  </si>
-  <si>
-    <t>foreigners</t>
-  </si>
-  <si>
-    <t>more intelligent</t>
-  </si>
-  <si>
-    <t>not as intelligent as</t>
-  </si>
-  <si>
-    <t>dumber</t>
-  </si>
-  <si>
-    <t>wiser</t>
-  </si>
-  <si>
-    <t>sharper</t>
-  </si>
-  <si>
-    <t>less stupid</t>
-  </si>
-  <si>
-    <t>less wise</t>
-  </si>
-  <si>
-    <t>less sharp</t>
-  </si>
-  <si>
-    <t>more backward</t>
-  </si>
-  <si>
-    <t>less astute</t>
-  </si>
-  <si>
-    <t>smarter</t>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Thank you, the task is now complete. Please contact the researcher.</t>
   </si>
@@ -197,7 +88,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -217,13 +108,6 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -339,10 +223,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -780,37 +662,37 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="195">
-      <c r="A2" s="3" t="s">
-        <v>37</v>
+      <c r="A2" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="300">
-      <c r="A3" s="3" t="s">
-        <v>39</v>
+      <c r="A3" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="315">
-      <c r="A4" s="3" t="s">
-        <v>40</v>
+      <c r="A4" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="285">
-      <c r="A5" s="3" t="s">
-        <v>41</v>
+      <c r="A5" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="255">
-      <c r="A6" s="3" t="s">
-        <v>38</v>
+      <c r="A6" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="3" t="s">
-        <v>36</v>
+      <c r="A7" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -822,389 +704,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="2" width="61.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="D26" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>